<commit_message>
ft: added med champ && initial testing
</commit_message>
<xml_diff>
--- a/data/campeonato_prueba_10eq.xlsx
+++ b/data/campeonato_prueba_10eq.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nico_7/Desktop/calendar-opt-development/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdduarte/Development/universidad/tesis/calendar-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D0E07A-E044-8E42-8F6F-6744BA3FE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D37E8F1-6178-1B46-9D71-DC3A8ABDD0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="38">
   <si>
     <t>EQUIPO</t>
   </si>
@@ -119,36 +119,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>RM</t>
-  </si>
-  <si>
-    <t>FEY</t>
-  </si>
-  <si>
-    <t>RCS</t>
-  </si>
-  <si>
-    <t>LIL</t>
-  </si>
-  <si>
-    <t>SLB</t>
-  </si>
-  <si>
-    <t>RIV</t>
-  </si>
-  <si>
-    <t>CEL</t>
-  </si>
-  <si>
-    <t>MIL</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
     <t>4 : 1</t>
   </si>
   <si>
@@ -175,12 +145,15 @@
   <si>
     <t>3 : 0</t>
   </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,10 +172,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -231,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,13 +209,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +433,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -499,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3">
         <v>21</v>
@@ -516,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
@@ -533,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <v>14</v>
@@ -550,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3">
         <v>5</v>
@@ -567,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3">
         <v>13</v>
@@ -584,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <v>14</v>
@@ -597,16 +565,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="5">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>4</v>
       </c>
     </row>
@@ -614,16 +582,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4">
         <v>15</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>5</v>
       </c>
     </row>
@@ -631,16 +599,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="5">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4">
         <v>15</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
     </row>
@@ -648,48 +616,48 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="5">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4">
         <v>6</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D18" s="2"/>
@@ -3651,7 +3619,7 @@
   <dimension ref="A1:E1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3677,650 +3645,766 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>46</v>
+      <c r="E9" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>44</v>
+      <c r="E15" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
+      <c r="E16" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>41</v>
+      <c r="E17" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
+      <c r="E18" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>45</v>
+      <c r="E19" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>41</v>
+      <c r="E23" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="C27" s="6" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>43</v>
+      <c r="E28" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="5"/>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>42</v>
+      <c r="E34" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>42</v>
+      <c r="E37" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="C39" s="6" t="s">
+      <c r="A39" s="5"/>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="C40" s="6" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>41</v>
+      <c r="E40" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
+      <c r="A44" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="6"/>
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6" t="s">
+      <c r="B46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>40</v>
+      <c r="E46" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="6"/>
-      <c r="C47" s="6" t="s">
+      <c r="B47" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6" t="s">
+      <c r="B48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+      <c r="A50" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6" t="s">
+      <c r="B51" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="6"/>
-      <c r="C52" s="6" t="s">
+      <c r="B52" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>39</v>
+      <c r="E52" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6" t="s">
+      <c r="B53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="6"/>
-      <c r="C54" s="6" t="s">
+      <c r="B54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6" t="s">
+      <c r="B55" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>40</v>
+      <c r="E55" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
+      <c r="A56" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="6"/>
-      <c r="C57" s="6" t="s">
+      <c r="B57" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="6"/>
-      <c r="C58" s="6" t="s">
+      <c r="B58" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>38</v>
+      <c r="E58" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="6"/>
-      <c r="C59" s="6" t="s">
+      <c r="B59" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C60" s="6" t="s">
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="6" t="s">
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rf: remove generate win patterns && sstpa normal working
</commit_message>
<xml_diff>
--- a/data/campeonato_prueba_10eq.xlsx
+++ b/data/campeonato_prueba_10eq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdduarte/Development/universidad/tesis/calendar-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D37E8F1-6178-1B46-9D71-DC3A8ABDD0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6DB4E-8686-404D-82DA-32B66616239A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="39">
   <si>
     <t>EQUIPO</t>
   </si>
@@ -146,14 +146,17 @@
     <t>3 : 0</t>
   </si>
   <si>
-    <t>n</t>
+    <t>2 :0</t>
+  </si>
+  <si>
+    <t>3 : 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,11 +176,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -213,8 +211,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
@@ -3618,8 +3614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3646,819 +3642,1175 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
+      <c r="E7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
+      <c r="E9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>34</v>
+      <c r="E15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>31</v>
+      <c r="E17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>35</v>
+      <c r="E19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
       <c r="C22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>20</v>
+      <c r="E25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
       <c r="C27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
       <c r="C28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>17</v>
+      <c r="E30" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>18</v>
+      <c r="E31" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
       <c r="C34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>32</v>
+      <c r="E37" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>22</v>
+      <c r="E39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="7" t="s">
+      <c r="E43" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>30</v>
+      <c r="E46" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>20</v>
+      <c r="E48" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>18</v>
+      <c r="E51" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D53" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="5" t="s">
+      <c r="A57" s="5"/>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>28</v>
+      <c r="E58" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>23</v>
+      <c r="E59" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>37</v>
-      </c>
+      <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>37</v>
-      </c>
+      <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="D67" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="5"/>
+      <c r="C82" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="5"/>
+      <c r="C85" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E100" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E103" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E109" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>